<commit_message>
added a row for the 2G model
</commit_message>
<xml_diff>
--- a/Test/C780_Incoming_product_checklist.xlsx
+++ b/Test/C780_Incoming_product_checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WiFi" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
   <si>
     <t xml:space="preserve">Object to check </t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">FW versions is the right one? </t>
+  </si>
+  <si>
+    <t>Only one antenna connector ?</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
@@ -575,13 +578,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="9" ySplit="14" topLeftCell="J15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,6 +663,11 @@
         <v>12</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
revised for the Design Freeze
</commit_message>
<xml_diff>
--- a/Test/C780_Incoming_product_checklist.xlsx
+++ b/Test/C780_Incoming_product_checklist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t xml:space="preserve">Object to check </t>
   </si>
@@ -83,6 +83,10 @@
   </si>
   <si>
     <t>Only one antenna connector ?</t>
+  </si>
+  <si>
+    <t>Are the SIM card installed ?
+test indirectly with the aid of the led</t>
   </si>
 </sst>
 </file>
@@ -578,7 +582,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="9" ySplit="14" topLeftCell="J15" activePane="bottomRight" state="frozen"/>
@@ -590,6 +594,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -668,6 +673,11 @@
         <v>21</v>
       </c>
     </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>